<commit_message>
it works ... somehow
</commit_message>
<xml_diff>
--- a/UPR/example/test_book.xlsx
+++ b/UPR/example/test_book.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>BLOCK TYPE</t>
   </si>
@@ -25,19 +25,22 @@
     <t>tag</t>
   </si>
   <si>
-    <t>Low EGU limit</t>
+    <t>Shelve policy</t>
+  </si>
+  <si>
+    <t>DI</t>
+  </si>
+  <si>
+    <t>bf2</t>
+  </si>
+  <si>
+    <t>vaf2</t>
+  </si>
+  <si>
+    <t>adada</t>
   </si>
   <si>
     <t>AI</t>
-  </si>
-  <si>
-    <t>bf2</t>
-  </si>
-  <si>
-    <t>vaf2</t>
-  </si>
-  <si>
-    <t>adada</t>
   </si>
   <si>
     <t>var4</t>
@@ -501,27 +504,27 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4" s="4">
         <v>51</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2">
         <v>65.6666666666667</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>7</v>
@@ -529,44 +532,44 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2">
         <v>79.1666666666667</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2">
         <v>92.6666666666667</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2">
         <v>106.166666666667</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ψ(._. )>   added comments
</commit_message>
<xml_diff>
--- a/UPR/example/test_book.xlsx
+++ b/UPR/example/test_book.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>BLOCK TYPE</t>
   </si>
@@ -25,6 +25,9 @@
     <t>Description</t>
   </si>
   <si>
+    <t>I/O device</t>
+  </si>
+  <si>
     <t>I/O address</t>
   </si>
   <si>
@@ -37,16 +40,25 @@
     <t>something something aaa</t>
   </si>
   <si>
+    <t>IAS</t>
+  </si>
+  <si>
     <t>AO</t>
   </si>
   <si>
     <t>ANALOG_OUTPUT</t>
   </si>
   <si>
+    <t>SSIM</t>
+  </si>
+  <si>
     <t>DI</t>
   </si>
   <si>
     <t>T</t>
+  </si>
+  <si>
+    <t>AA</t>
   </si>
   <si>
     <t>1:1</t>
@@ -66,7 +78,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +89,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -108,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -116,14 +134,20 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -427,16 +451,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -452,61 +477,74 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4">
         <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="3">
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>